<commit_message>
Fixed off-by-one errors caused by misunderstanding of python range. Added Bowling Green.
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jazzman/Dropbox/dev/trip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syd/Dropbox/dev/trip/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27340" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="trip.tab" sheetId="1" r:id="rId1"/>
     <sheet name="Like cities" sheetId="2" r:id="rId2"/>
     <sheet name="distances.txt" sheetId="3" r:id="rId3"/>
-    <sheet name="master.txt" sheetId="4" r:id="rId4"/>
+    <sheet name="wait_times.txt" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="59">
   <si>
     <t>San Diego</t>
   </si>
@@ -217,12 +217,15 @@
   <si>
     <t>New York</t>
   </si>
+  <si>
+    <t>Bowling Green</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -245,6 +248,18 @@
       <sz val="8"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -263,8 +278,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -277,7 +294,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -50488,13 +50507,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT46"/>
+  <dimension ref="A1:AR44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B47" sqref="B47"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -50536,20 +50555,17 @@
     <col min="35" max="35" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A1" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
@@ -50660,34 +50676,28 @@
         <v>56</v>
       </c>
       <c r="AL1" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="AM1" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AN1" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AO1" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AP1" s="5" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="AQ1" s="5" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="AR1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT1" s="5" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -50800,34 +50810,28 @@
         <v>26</v>
       </c>
       <c r="AL2" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AM2" s="5">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="AN2" s="5">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="AO2" s="5">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="AP2" s="5">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AQ2" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AR2" s="5">
-        <v>31</v>
-      </c>
-      <c r="AS2" s="5">
-        <v>20</v>
-      </c>
-      <c r="AT2" s="5">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -50940,34 +50944,28 @@
         <v>49</v>
       </c>
       <c r="AL3" s="5">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="AM3" s="5">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AN3" s="5">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="AO3" s="5">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="AP3" s="5">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="AQ3" s="5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AR3" s="5">
-        <v>49</v>
-      </c>
-      <c r="AS3" s="5">
-        <v>7</v>
-      </c>
-      <c r="AT3" s="5">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -51080,34 +51078,28 @@
         <v>49</v>
       </c>
       <c r="AL4" s="5">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="AM4" s="5">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AN4" s="5">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="AO4" s="5">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="AP4" s="5">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="AQ4" s="5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AR4" s="5">
-        <v>49</v>
-      </c>
-      <c r="AS4" s="5">
-        <v>7</v>
-      </c>
-      <c r="AT4" s="5">
-        <v>49</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -51220,34 +51212,28 @@
         <v>48</v>
       </c>
       <c r="AL5" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AM5" s="5">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AN5" s="5">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="AO5" s="5">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="AP5" s="5">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="AQ5" s="5">
         <v>43</v>
       </c>
       <c r="AR5" s="5">
-        <v>47</v>
-      </c>
-      <c r="AS5" s="5">
-        <v>1</v>
-      </c>
-      <c r="AT5" s="5">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -51360,34 +51346,28 @@
         <v>48</v>
       </c>
       <c r="AL6" s="5">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AM6" s="5">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AN6" s="5">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="AO6" s="5">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="AP6" s="5">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="5">
         <v>43</v>
       </c>
       <c r="AR6" s="5">
-        <v>47</v>
-      </c>
-      <c r="AS6" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="5">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -51500,34 +51480,28 @@
         <v>46</v>
       </c>
       <c r="AL7" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AM7" s="5">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="AN7" s="5">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="AO7" s="5">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="AP7" s="5">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="AQ7" s="5">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AR7" s="5">
-        <v>48</v>
-      </c>
-      <c r="AS7" s="5">
-        <v>2</v>
-      </c>
-      <c r="AT7" s="5">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -51643,31 +51617,25 @@
         <v>30</v>
       </c>
       <c r="AM8" s="5">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="AN8" s="5">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="AO8" s="5">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="AP8" s="5">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="AQ8" s="5">
         <v>38</v>
       </c>
       <c r="AR8" s="5">
-        <v>43</v>
-      </c>
-      <c r="AS8" s="5">
-        <v>6</v>
-      </c>
-      <c r="AT8" s="5">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -51780,34 +51748,28 @@
         <v>30</v>
       </c>
       <c r="AL9" s="5">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="AM9" s="5">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="AN9" s="5">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="AO9" s="5">
+        <v>30</v>
+      </c>
+      <c r="AP9" s="5">
+        <v>15</v>
+      </c>
+      <c r="AQ9" s="5">
+        <v>32</v>
+      </c>
+      <c r="AR9" s="5">
         <v>14</v>
       </c>
-      <c r="AP9" s="5">
-        <v>22</v>
-      </c>
-      <c r="AQ9" s="5">
-        <v>29</v>
-      </c>
-      <c r="AR9" s="5">
-        <v>30</v>
-      </c>
-      <c r="AS9" s="5">
-        <v>15</v>
-      </c>
-      <c r="AT9" s="5">
-        <v>32</v>
-      </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -51920,34 +51882,28 @@
         <v>19</v>
       </c>
       <c r="AL10" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="AM10" s="5">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="AN10" s="5">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="AO10" s="5">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="AP10" s="5">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="AQ10" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="AR10" s="5">
-        <v>21</v>
-      </c>
-      <c r="AS10" s="5">
-        <v>25</v>
-      </c>
-      <c r="AT10" s="5">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -52060,34 +52016,28 @@
         <v>24</v>
       </c>
       <c r="AL11" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AM11" s="5">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AN11" s="5">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="AO11" s="5">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="AP11" s="5">
         <v>21</v>
       </c>
       <c r="AQ11" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AR11" s="5">
-        <v>27</v>
-      </c>
-      <c r="AS11" s="5">
-        <v>21</v>
-      </c>
-      <c r="AT11" s="5">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -52200,34 +52150,28 @@
         <v>15</v>
       </c>
       <c r="AL12" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AM12" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AN12" s="5">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AO12" s="5">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="AP12" s="5">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="AQ12" s="5">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="AR12" s="5">
-        <v>16</v>
-      </c>
-      <c r="AS12" s="5">
-        <v>30</v>
-      </c>
-      <c r="AT12" s="5">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -52340,34 +52284,28 @@
         <v>14</v>
       </c>
       <c r="AL13" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AM13" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN13" s="5">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AO13" s="5">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="AP13" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="AQ13" s="5">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AR13" s="5">
-        <v>14</v>
-      </c>
-      <c r="AS13" s="5">
-        <v>30</v>
-      </c>
-      <c r="AT13" s="5">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -52480,34 +52418,28 @@
         <v>14</v>
       </c>
       <c r="AL14" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AM14" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN14" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AO14" s="5">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="AP14" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="AQ14" s="5">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="AR14" s="5">
-        <v>14</v>
-      </c>
-      <c r="AS14" s="5">
-        <v>30</v>
-      </c>
-      <c r="AT14" s="5">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -52620,34 +52552,28 @@
         <v>7</v>
       </c>
       <c r="AL15" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AM15" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AN15" s="5">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="AO15" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AP15" s="5">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="AQ15" s="5">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="AR15" s="5">
         <v>7</v>
       </c>
-      <c r="AS15" s="5">
-        <v>34</v>
-      </c>
-      <c r="AT15" s="5">
-        <v>18</v>
-      </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -52760,34 +52686,28 @@
         <v>0</v>
       </c>
       <c r="AL16" s="5">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="AM16" s="5">
         <v>11</v>
       </c>
       <c r="AN16" s="5">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="AO16" s="5">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="AP16" s="5">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="AQ16" s="5">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="AR16" s="5">
-        <v>6</v>
-      </c>
-      <c r="AS16" s="5">
-        <v>42</v>
-      </c>
-      <c r="AT16" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -52900,34 +52820,28 @@
         <v>0</v>
       </c>
       <c r="AL17" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AM17" s="5">
         <v>11</v>
       </c>
       <c r="AN17" s="5">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="AO17" s="5">
+        <v>7</v>
+      </c>
+      <c r="AP17" s="5">
+        <v>40</v>
+      </c>
+      <c r="AQ17" s="5">
         <v>15</v>
       </c>
-      <c r="AP17" s="5">
-        <v>11</v>
-      </c>
-      <c r="AQ17" s="5">
-        <v>5</v>
-      </c>
       <c r="AR17" s="5">
-        <v>7</v>
-      </c>
-      <c r="AS17" s="5">
-        <v>40</v>
-      </c>
-      <c r="AT17" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -53040,34 +52954,28 @@
         <v>9</v>
       </c>
       <c r="AL18" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AM18" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AN18" s="5">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="AO18" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AP18" s="5">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="AQ18" s="5">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="AR18" s="5">
-        <v>9</v>
-      </c>
-      <c r="AS18" s="5">
-        <v>33</v>
-      </c>
-      <c r="AT18" s="5">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -53180,34 +53088,28 @@
         <v>9</v>
       </c>
       <c r="AL19" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AM19" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AN19" s="5">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AO19" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AP19" s="5">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="AQ19" s="5">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="AR19" s="5">
-        <v>11</v>
-      </c>
-      <c r="AS19" s="5">
-        <v>31</v>
-      </c>
-      <c r="AT19" s="5">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -53320,34 +53222,28 @@
         <v>22</v>
       </c>
       <c r="AL20" s="5">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AM20" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AN20" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="AO20" s="5">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="AP20" s="5">
+        <v>28</v>
+      </c>
+      <c r="AQ20" s="5">
+        <v>27</v>
+      </c>
+      <c r="AR20" s="5">
         <v>13</v>
       </c>
-      <c r="AQ20" s="5">
-        <v>22</v>
-      </c>
-      <c r="AR20" s="5">
-        <v>22</v>
-      </c>
-      <c r="AS20" s="5">
-        <v>28</v>
-      </c>
-      <c r="AT20" s="5">
-        <v>27</v>
-      </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -53460,34 +53356,28 @@
         <v>9</v>
       </c>
       <c r="AL21" s="5">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AM21" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AN21" s="5">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="AO21" s="5">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="AP21" s="5">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="AQ21" s="5">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="AR21" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS21" s="5">
-        <v>45</v>
-      </c>
-      <c r="AT21" s="5">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -53600,34 +53490,28 @@
         <v>5</v>
       </c>
       <c r="AL22" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AM22" s="5">
         <v>7</v>
       </c>
       <c r="AN22" s="5">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="AO22" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AP22" s="5">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="AQ22" s="5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="AR22" s="5">
         <v>7</v>
       </c>
-      <c r="AS22" s="5">
-        <v>35</v>
-      </c>
-      <c r="AT22" s="5">
-        <v>17</v>
-      </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -53740,34 +53624,28 @@
         <v>15</v>
       </c>
       <c r="AL23" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AM23" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AN23" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AO23" s="5">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="AP23" s="5">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="AQ23" s="5">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AR23" s="5">
-        <v>17</v>
-      </c>
-      <c r="AS23" s="5">
-        <v>27</v>
-      </c>
-      <c r="AT23" s="5">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -53880,34 +53758,28 @@
         <v>12</v>
       </c>
       <c r="AL24" s="5">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="AM24" s="5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="AN24" s="5">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="AO24" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AP24" s="5">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="AQ24" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AR24" s="5">
-        <v>16</v>
-      </c>
-      <c r="AS24" s="5">
-        <v>32</v>
-      </c>
-      <c r="AT24" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -54020,34 +53892,28 @@
         <v>18</v>
       </c>
       <c r="AL25" s="5">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="AM25" s="5">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="AN25" s="5">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="AO25" s="5">
         <v>24</v>
       </c>
       <c r="AP25" s="5">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="AQ25" s="5">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="AR25" s="5">
-        <v>24</v>
-      </c>
-      <c r="AS25" s="5">
-        <v>40</v>
-      </c>
-      <c r="AT25" s="5">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -54160,34 +54026,28 @@
         <v>16</v>
       </c>
       <c r="AL26" s="5">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="AM26" s="5">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AN26" s="5">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="AO26" s="5">
         <v>22</v>
       </c>
       <c r="AP26" s="5">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="AQ26" s="5">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="AR26" s="5">
-        <v>22</v>
-      </c>
-      <c r="AS26" s="5">
-        <v>37</v>
-      </c>
-      <c r="AT26" s="5">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -54300,34 +54160,28 @@
         <v>25</v>
       </c>
       <c r="AL27" s="5">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="AM27" s="5">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="AN27" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AO27" s="5">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="AP27" s="5">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AQ27" s="5">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AR27" s="5">
-        <v>28</v>
-      </c>
-      <c r="AS27" s="5">
-        <v>21</v>
-      </c>
-      <c r="AT27" s="5">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -54440,34 +54294,28 @@
         <v>2</v>
       </c>
       <c r="AL28" s="5">
+        <v>15</v>
+      </c>
+      <c r="AM28" s="5">
+        <v>12</v>
+      </c>
+      <c r="AN28" s="5">
+        <v>7</v>
+      </c>
+      <c r="AO28" s="5">
+        <v>5</v>
+      </c>
+      <c r="AP28" s="5">
+        <v>40</v>
+      </c>
+      <c r="AQ28" s="5">
+        <v>17</v>
+      </c>
+      <c r="AR28" s="5">
         <v>11</v>
       </c>
-      <c r="AM28" s="5">
-        <v>11</v>
-      </c>
-      <c r="AN28" s="5">
-        <v>27</v>
-      </c>
-      <c r="AO28" s="5">
-        <v>15</v>
-      </c>
-      <c r="AP28" s="5">
-        <v>12</v>
-      </c>
-      <c r="AQ28" s="5">
-        <v>7</v>
-      </c>
-      <c r="AR28" s="5">
-        <v>5</v>
-      </c>
-      <c r="AS28" s="5">
-        <v>40</v>
-      </c>
-      <c r="AT28" s="5">
-        <v>17</v>
-      </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
@@ -54580,34 +54428,28 @@
         <v>5</v>
       </c>
       <c r="AL29" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM29" s="5">
         <v>12</v>
       </c>
-      <c r="AM29" s="5">
+      <c r="AN29" s="5">
+        <v>9</v>
+      </c>
+      <c r="AO29" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP29" s="5">
+        <v>41</v>
+      </c>
+      <c r="AQ29" s="5">
+        <v>19</v>
+      </c>
+      <c r="AR29" s="5">
         <v>13</v>
       </c>
-      <c r="AN29" s="5">
-        <v>28</v>
-      </c>
-      <c r="AO29" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP29" s="5">
-        <v>12</v>
-      </c>
-      <c r="AQ29" s="5">
-        <v>9</v>
-      </c>
-      <c r="AR29" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS29" s="5">
-        <v>41</v>
-      </c>
-      <c r="AT29" s="5">
-        <v>19</v>
-      </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
@@ -54720,34 +54562,28 @@
         <v>5</v>
       </c>
       <c r="AL30" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM30" s="5">
         <v>12</v>
       </c>
-      <c r="AM30" s="5">
+      <c r="AN30" s="5">
+        <v>9</v>
+      </c>
+      <c r="AO30" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP30" s="5">
+        <v>41</v>
+      </c>
+      <c r="AQ30" s="5">
+        <v>19</v>
+      </c>
+      <c r="AR30" s="5">
         <v>13</v>
       </c>
-      <c r="AN30" s="5">
-        <v>28</v>
-      </c>
-      <c r="AO30" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP30" s="5">
-        <v>12</v>
-      </c>
-      <c r="AQ30" s="5">
-        <v>9</v>
-      </c>
-      <c r="AR30" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS30" s="5">
-        <v>41</v>
-      </c>
-      <c r="AT30" s="5">
-        <v>19</v>
-      </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -54860,34 +54696,28 @@
         <v>9</v>
       </c>
       <c r="AL31" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AM31" s="5">
+        <v>6</v>
+      </c>
+      <c r="AN31" s="5">
+        <v>13</v>
+      </c>
+      <c r="AO31" s="5">
+        <v>6</v>
+      </c>
+      <c r="AP31" s="5">
+        <v>37</v>
+      </c>
+      <c r="AQ31" s="5">
+        <v>22</v>
+      </c>
+      <c r="AR31" s="5">
         <v>10</v>
       </c>
-      <c r="AN31" s="5">
-        <v>26</v>
-      </c>
-      <c r="AO31" s="5">
-        <v>12</v>
-      </c>
-      <c r="AP31" s="5">
-        <v>6</v>
-      </c>
-      <c r="AQ31" s="5">
-        <v>13</v>
-      </c>
-      <c r="AR31" s="5">
-        <v>6</v>
-      </c>
-      <c r="AS31" s="5">
-        <v>37</v>
-      </c>
-      <c r="AT31" s="5">
-        <v>22</v>
-      </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
@@ -55000,34 +54830,28 @@
         <v>48</v>
       </c>
       <c r="AL32" s="5">
+        <v>31</v>
+      </c>
+      <c r="AM32" s="5">
         <v>40</v>
       </c>
-      <c r="AM32" s="5">
-        <v>37</v>
-      </c>
       <c r="AN32" s="5">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="AO32" s="5">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="AP32" s="5">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="AQ32" s="5">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="AR32" s="5">
-        <v>49</v>
-      </c>
-      <c r="AS32" s="5">
-        <v>19</v>
-      </c>
-      <c r="AT32" s="5">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
         <v>53</v>
       </c>
@@ -55140,34 +54964,28 @@
         <v>49</v>
       </c>
       <c r="AL33" s="5">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="AM33" s="5">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AN33" s="5">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="AO33" s="5">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="AP33" s="5">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="AQ33" s="5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AR33" s="5">
-        <v>49</v>
-      </c>
-      <c r="AS33" s="5">
-        <v>7</v>
-      </c>
-      <c r="AT33" s="5">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
         <v>54</v>
       </c>
@@ -55280,34 +55098,28 @@
         <v>48</v>
       </c>
       <c r="AL34" s="5">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AM34" s="5">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AN34" s="5">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="AO34" s="5">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="AP34" s="5">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="AQ34" s="5">
         <v>43</v>
       </c>
       <c r="AR34" s="5">
-        <v>47</v>
-      </c>
-      <c r="AS34" s="5">
-        <v>1</v>
-      </c>
-      <c r="AT34" s="5">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
         <v>55</v>
       </c>
@@ -55420,34 +55232,28 @@
         <v>14</v>
       </c>
       <c r="AL35" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AM35" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN35" s="5">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AO35" s="5">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="AP35" s="5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="AQ35" s="5">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="AR35" s="5">
-        <v>14</v>
-      </c>
-      <c r="AS35" s="5">
-        <v>30</v>
-      </c>
-      <c r="AT35" s="5">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>57</v>
       </c>
@@ -55560,34 +55366,28 @@
         <v>5</v>
       </c>
       <c r="AL36" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM36" s="5">
         <v>12</v>
       </c>
-      <c r="AM36" s="5">
+      <c r="AN36" s="5">
+        <v>9</v>
+      </c>
+      <c r="AO36" s="5">
+        <v>4</v>
+      </c>
+      <c r="AP36" s="5">
+        <v>41</v>
+      </c>
+      <c r="AQ36" s="5">
+        <v>19</v>
+      </c>
+      <c r="AR36" s="5">
         <v>13</v>
       </c>
-      <c r="AN36" s="5">
-        <v>28</v>
-      </c>
-      <c r="AO36" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP36" s="5">
-        <v>12</v>
-      </c>
-      <c r="AQ36" s="5">
-        <v>9</v>
-      </c>
-      <c r="AR36" s="5">
-        <v>4</v>
-      </c>
-      <c r="AS36" s="5">
-        <v>41</v>
-      </c>
-      <c r="AT36" s="5">
-        <v>19</v>
-      </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
         <v>56</v>
       </c>
@@ -55700,859 +55500,823 @@
         <v>0</v>
       </c>
       <c r="AL37" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AM37" s="5">
         <v>11</v>
       </c>
       <c r="AN37" s="5">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="AO37" s="5">
+        <v>7</v>
+      </c>
+      <c r="AP37" s="5">
+        <v>42</v>
+      </c>
+      <c r="AQ37" s="5">
         <v>15</v>
       </c>
-      <c r="AP37" s="5">
-        <v>11</v>
-      </c>
-      <c r="AQ37" s="5">
-        <v>5</v>
-      </c>
       <c r="AR37" s="5">
-        <v>7</v>
-      </c>
-      <c r="AS37" s="5">
-        <v>42</v>
-      </c>
-      <c r="AT37" s="5">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="1">
+        <v>18</v>
+      </c>
+      <c r="C38" s="1">
+        <v>39</v>
+      </c>
+      <c r="D38" s="1">
+        <v>30</v>
+      </c>
+      <c r="E38" s="1">
+        <v>28</v>
+      </c>
+      <c r="F38" s="1">
         <v>27</v>
       </c>
-      <c r="B38" s="1">
-        <v>16</v>
-      </c>
-      <c r="C38" s="1">
-        <v>35</v>
-      </c>
-      <c r="D38" s="1">
-        <v>35</v>
-      </c>
-      <c r="E38" s="1">
-        <v>31</v>
-      </c>
-      <c r="F38" s="1">
-        <v>31</v>
-      </c>
       <c r="G38" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H38" s="1">
         <v>26</v>
       </c>
       <c r="I38" s="1">
+        <v>12</v>
+      </c>
+      <c r="J38" s="1">
+        <v>6</v>
+      </c>
+      <c r="K38" s="1">
+        <v>15</v>
+      </c>
+      <c r="L38" s="1">
+        <v>4</v>
+      </c>
+      <c r="M38" s="1">
+        <v>4</v>
+      </c>
+      <c r="N38" s="1">
+        <v>4</v>
+      </c>
+      <c r="O38" s="1">
+        <v>10</v>
+      </c>
+      <c r="P38" s="5">
+        <v>16</v>
+      </c>
+      <c r="Q38" s="5">
         <v>17</v>
       </c>
-      <c r="J38" s="1">
-        <v>9</v>
-      </c>
-      <c r="K38" s="1">
+      <c r="R38" s="5">
+        <v>10</v>
+      </c>
+      <c r="S38" s="5">
+        <v>10</v>
+      </c>
+      <c r="T38" s="5">
+        <v>5</v>
+      </c>
+      <c r="U38" s="5">
+        <v>21</v>
+      </c>
+      <c r="V38" s="5">
         <v>12</v>
       </c>
-      <c r="L38" s="1">
-        <v>8</v>
-      </c>
-      <c r="M38" s="1">
-        <v>7</v>
-      </c>
-      <c r="N38" s="1">
-        <v>6</v>
-      </c>
-      <c r="O38" s="1">
-        <v>6</v>
-      </c>
-      <c r="P38" s="5">
-        <v>12</v>
-      </c>
-      <c r="Q38" s="5">
-        <v>12</v>
-      </c>
-      <c r="R38" s="5">
-        <v>9</v>
-      </c>
-      <c r="S38" s="5">
-        <v>4</v>
-      </c>
-      <c r="T38" s="5">
+      <c r="W38" s="5">
+        <v>6</v>
+      </c>
+      <c r="X38" s="5">
         <v>16</v>
       </c>
-      <c r="U38" s="5">
+      <c r="Y38" s="5">
+        <v>26</v>
+      </c>
+      <c r="Z38" s="5">
+        <v>24</v>
+      </c>
+      <c r="AA38" s="5">
+        <v>19</v>
+      </c>
+      <c r="AB38" s="5">
+        <v>17</v>
+      </c>
+      <c r="AC38" s="5">
         <v>18</v>
       </c>
-      <c r="V38" s="5">
-        <v>8</v>
-      </c>
-      <c r="W38" s="5">
-        <v>4</v>
-      </c>
-      <c r="X38" s="5">
-        <v>7</v>
-      </c>
-      <c r="Y38" s="5">
+      <c r="AD38" s="5">
         <v>18</v>
       </c>
-      <c r="Z38" s="5">
-        <v>15</v>
-      </c>
-      <c r="AA38" s="5">
-        <v>15</v>
-      </c>
-      <c r="AB38" s="5">
-        <v>13</v>
-      </c>
-      <c r="AC38" s="5">
+      <c r="AE38" s="5">
         <v>14</v>
       </c>
-      <c r="AD38" s="5">
-        <v>14</v>
-      </c>
-      <c r="AE38" s="5">
-        <v>13</v>
-      </c>
       <c r="AF38" s="5">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="AG38" s="5">
+        <v>30</v>
+      </c>
+      <c r="AH38" s="5">
+        <v>28</v>
+      </c>
+      <c r="AI38" s="5">
+        <v>4</v>
+      </c>
+      <c r="AJ38" s="5">
+        <v>18</v>
+      </c>
+      <c r="AK38" s="5">
+        <v>17</v>
+      </c>
+      <c r="AL38" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM38" s="5">
+        <v>9</v>
+      </c>
+      <c r="AN38" s="5">
+        <v>18</v>
+      </c>
+      <c r="AO38" s="5">
+        <v>18</v>
+      </c>
+      <c r="AP38" s="5">
+        <v>26</v>
+      </c>
+      <c r="AQ38" s="5">
+        <v>23</v>
+      </c>
+      <c r="AR38" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="1">
+        <v>22</v>
+      </c>
+      <c r="C39" s="1">
+        <v>34</v>
+      </c>
+      <c r="D39" s="1">
         <v>35</v>
       </c>
-      <c r="AH38" s="5">
-        <v>31</v>
-      </c>
-      <c r="AI38" s="5">
-        <v>7</v>
-      </c>
-      <c r="AJ38" s="5">
-        <v>14</v>
-      </c>
-      <c r="AK38" s="5">
-        <v>12</v>
-      </c>
-      <c r="AL38" s="5">
-        <v>0</v>
-      </c>
-      <c r="AM38" s="5">
-        <v>3</v>
-      </c>
-      <c r="AN38" s="5">
-        <v>17</v>
-      </c>
-      <c r="AO38" s="5">
-        <v>10</v>
-      </c>
-      <c r="AP38" s="5">
-        <v>9</v>
-      </c>
-      <c r="AQ38" s="5">
+      <c r="E39" s="1">
+        <v>33</v>
+      </c>
+      <c r="F39" s="1">
+        <v>33</v>
+      </c>
+      <c r="G39" s="1">
+        <v>34</v>
+      </c>
+      <c r="H39" s="1">
+        <v>29</v>
+      </c>
+      <c r="I39" s="1">
+        <v>18</v>
+      </c>
+      <c r="J39" s="1">
         <v>11</v>
       </c>
-      <c r="AR38" s="5">
-        <v>15</v>
-      </c>
-      <c r="AS38" s="5">
-        <v>30</v>
-      </c>
-      <c r="AT38" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="1">
-        <v>17</v>
-      </c>
-      <c r="C39" s="1">
-        <v>33</v>
-      </c>
-      <c r="D39" s="1">
-        <v>33</v>
-      </c>
-      <c r="E39" s="1">
-        <v>30</v>
-      </c>
-      <c r="F39" s="1">
-        <v>30</v>
-      </c>
-      <c r="G39" s="1">
-        <v>30</v>
-      </c>
-      <c r="H39" s="1">
-        <v>25</v>
-      </c>
-      <c r="I39" s="1">
-        <v>15</v>
-      </c>
-      <c r="J39" s="1">
-        <v>7</v>
-      </c>
       <c r="K39" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="L39" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O39" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="P39" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Q39" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R39" s="5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="S39" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="T39" s="5">
         <v>11</v>
       </c>
       <c r="U39" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="V39" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="W39" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="X39" s="5">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="Y39" s="5">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="Z39" s="5">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="AA39" s="5">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AB39" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AC39" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AD39" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AE39" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="AF39" s="5">
         <v>34</v>
       </c>
       <c r="AG39" s="5">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AH39" s="5">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="AI39" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AJ39" s="5">
+        <v>12</v>
+      </c>
+      <c r="AK39" s="5">
+        <v>11</v>
+      </c>
+      <c r="AL39" s="5">
+        <v>7</v>
+      </c>
+      <c r="AM39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN39" s="5">
+        <v>14</v>
+      </c>
+      <c r="AO39" s="5">
+        <v>11</v>
+      </c>
+      <c r="AP39" s="5">
+        <v>33</v>
+      </c>
+      <c r="AQ39" s="5">
+        <v>22</v>
+      </c>
+      <c r="AR39" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="1">
+        <v>20</v>
+      </c>
+      <c r="C40" s="1">
+        <v>42</v>
+      </c>
+      <c r="D40" s="1">
+        <v>42</v>
+      </c>
+      <c r="E40" s="1">
+        <v>37</v>
+      </c>
+      <c r="F40" s="1">
+        <v>37</v>
+      </c>
+      <c r="G40" s="1">
+        <v>37</v>
+      </c>
+      <c r="H40" s="1">
+        <v>32</v>
+      </c>
+      <c r="I40" s="1">
+        <v>25</v>
+      </c>
+      <c r="J40" s="1">
+        <v>16</v>
+      </c>
+      <c r="K40" s="1">
+        <v>18</v>
+      </c>
+      <c r="L40" s="1">
+        <v>14</v>
+      </c>
+      <c r="M40" s="1">
+        <v>13</v>
+      </c>
+      <c r="N40" s="1">
+        <v>12</v>
+      </c>
+      <c r="O40" s="1">
+        <v>9</v>
+      </c>
+      <c r="P40" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>5</v>
+      </c>
+      <c r="R40" s="5">
+        <v>11</v>
+      </c>
+      <c r="S40" s="5">
+        <v>9</v>
+      </c>
+      <c r="T40" s="5">
+        <v>20</v>
+      </c>
+      <c r="U40" s="5">
+        <v>12</v>
+      </c>
+      <c r="V40" s="5">
+        <v>8</v>
+      </c>
+      <c r="W40" s="5">
+        <v>12</v>
+      </c>
+      <c r="X40" s="5">
+        <v>6</v>
+      </c>
+      <c r="Y40" s="5">
+        <v>13</v>
+      </c>
+      <c r="Z40" s="5">
+        <v>12</v>
+      </c>
+      <c r="AA40" s="5">
+        <v>18</v>
+      </c>
+      <c r="AB40" s="5">
+        <v>7</v>
+      </c>
+      <c r="AC40" s="5">
+        <v>9</v>
+      </c>
+      <c r="AD40" s="5">
+        <v>9</v>
+      </c>
+      <c r="AE40" s="5">
+        <v>13</v>
+      </c>
+      <c r="AF40" s="5">
+        <v>43</v>
+      </c>
+      <c r="AG40" s="5">
+        <v>42</v>
+      </c>
+      <c r="AH40" s="5">
+        <v>37</v>
+      </c>
+      <c r="AI40" s="5">
+        <v>13</v>
+      </c>
+      <c r="AJ40" s="5">
+        <v>9</v>
+      </c>
+      <c r="AK40" s="5">
+        <v>5</v>
+      </c>
+      <c r="AL40" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM40" s="5">
+        <v>14</v>
+      </c>
+      <c r="AN40" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO40" s="5">
+        <v>11</v>
+      </c>
+      <c r="AP40" s="5">
+        <v>37</v>
+      </c>
+      <c r="AQ40" s="5">
+        <v>11</v>
+      </c>
+      <c r="AR40" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="1">
+        <v>29</v>
+      </c>
+      <c r="C41" s="1">
+        <v>43</v>
+      </c>
+      <c r="D41" s="1">
+        <v>43</v>
+      </c>
+      <c r="E41" s="1">
+        <v>41</v>
+      </c>
+      <c r="F41" s="1">
+        <v>41</v>
+      </c>
+      <c r="G41" s="1">
+        <v>42</v>
+      </c>
+      <c r="H41" s="1">
+        <v>37</v>
+      </c>
+      <c r="I41" s="1">
+        <v>26</v>
+      </c>
+      <c r="J41" s="1">
+        <v>19</v>
+      </c>
+      <c r="K41" s="1">
+        <v>29</v>
+      </c>
+      <c r="L41" s="1">
+        <v>14</v>
+      </c>
+      <c r="M41" s="1">
+        <v>12</v>
+      </c>
+      <c r="N41" s="1">
+        <v>12</v>
+      </c>
+      <c r="O41" s="1">
+        <v>7</v>
+      </c>
+      <c r="P41" s="5">
+        <v>6</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>7</v>
+      </c>
+      <c r="R41" s="5">
+        <v>9</v>
+      </c>
+      <c r="S41" s="5">
+        <v>11</v>
+      </c>
+      <c r="T41" s="5">
+        <v>20</v>
+      </c>
+      <c r="U41" s="5">
+        <v>4</v>
+      </c>
+      <c r="V41" s="5">
+        <v>7</v>
+      </c>
+      <c r="W41" s="5">
         <v>15</v>
-      </c>
-      <c r="AK39" s="5">
-        <v>13</v>
-      </c>
-      <c r="AL39" s="5">
-        <v>3</v>
-      </c>
-      <c r="AM39" s="5">
-        <v>0</v>
-      </c>
-      <c r="AN39" s="5">
-        <v>16</v>
-      </c>
-      <c r="AO39" s="5">
-        <v>7</v>
-      </c>
-      <c r="AP39" s="5">
-        <v>8</v>
-      </c>
-      <c r="AQ39" s="5">
-        <v>13</v>
-      </c>
-      <c r="AR39" s="5">
-        <v>15</v>
-      </c>
-      <c r="AS39" s="5">
-        <v>29</v>
-      </c>
-      <c r="AT39" s="5">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="1">
-        <v>8</v>
-      </c>
-      <c r="C40" s="1">
-        <v>20</v>
-      </c>
-      <c r="D40" s="1">
-        <v>20</v>
-      </c>
-      <c r="E40" s="1">
-        <v>15</v>
-      </c>
-      <c r="F40" s="1">
-        <v>15</v>
-      </c>
-      <c r="G40" s="1">
-        <v>16</v>
-      </c>
-      <c r="H40" s="1">
-        <v>10</v>
-      </c>
-      <c r="I40" s="1">
-        <v>8</v>
-      </c>
-      <c r="J40" s="1">
-        <v>11</v>
-      </c>
-      <c r="K40" s="1">
-        <v>6</v>
-      </c>
-      <c r="L40" s="1">
-        <v>20</v>
-      </c>
-      <c r="M40" s="1">
-        <v>19</v>
-      </c>
-      <c r="N40" s="1">
-        <v>88</v>
-      </c>
-      <c r="O40" s="1">
-        <v>24</v>
-      </c>
-      <c r="P40" s="5">
-        <v>28</v>
-      </c>
-      <c r="Q40" s="5">
-        <v>28</v>
-      </c>
-      <c r="R40" s="5">
-        <v>26</v>
-      </c>
-      <c r="S40" s="5">
-        <v>20</v>
-      </c>
-      <c r="T40" s="5">
-        <v>18</v>
-      </c>
-      <c r="U40" s="5">
-        <v>34</v>
-      </c>
-      <c r="V40" s="5">
-        <v>24</v>
-      </c>
-      <c r="W40" s="5">
-        <v>13</v>
-      </c>
-      <c r="X40" s="5">
-        <v>20</v>
-      </c>
-      <c r="Y40" s="5">
-        <v>29</v>
-      </c>
-      <c r="Z40" s="5">
-        <v>26</v>
-      </c>
-      <c r="AA40" s="5">
-        <v>10</v>
-      </c>
-      <c r="AB40" s="5">
-        <v>29</v>
-      </c>
-      <c r="AC40" s="5">
-        <v>30</v>
-      </c>
-      <c r="AD40" s="5">
-        <v>30</v>
-      </c>
-      <c r="AE40" s="5">
-        <v>28</v>
-      </c>
-      <c r="AF40" s="5">
-        <v>27</v>
-      </c>
-      <c r="AG40" s="5">
-        <v>20</v>
-      </c>
-      <c r="AH40" s="5">
-        <v>15</v>
-      </c>
-      <c r="AI40" s="5">
-        <v>19</v>
-      </c>
-      <c r="AJ40" s="5">
-        <v>28</v>
-      </c>
-      <c r="AK40" s="5">
-        <v>28</v>
-      </c>
-      <c r="AL40" s="5">
-        <v>17</v>
-      </c>
-      <c r="AM40" s="5">
-        <v>16</v>
-      </c>
-      <c r="AN40" s="5">
-        <v>0</v>
-      </c>
-      <c r="AO40" s="5">
-        <v>17</v>
-      </c>
-      <c r="AP40" s="5">
-        <v>23</v>
-      </c>
-      <c r="AQ40" s="5">
-        <v>25</v>
-      </c>
-      <c r="AR40" s="5">
-        <v>31</v>
-      </c>
-      <c r="AS40" s="5">
-        <v>14</v>
-      </c>
-      <c r="AT40" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="1">
-        <v>18</v>
-      </c>
-      <c r="C41" s="1">
-        <v>39</v>
-      </c>
-      <c r="D41" s="1">
-        <v>30</v>
-      </c>
-      <c r="E41" s="1">
-        <v>28</v>
-      </c>
-      <c r="F41" s="1">
-        <v>27</v>
-      </c>
-      <c r="G41" s="1">
-        <v>28</v>
-      </c>
-      <c r="H41" s="1">
-        <v>26</v>
-      </c>
-      <c r="I41" s="1">
-        <v>12</v>
-      </c>
-      <c r="J41" s="1">
-        <v>6</v>
-      </c>
-      <c r="K41" s="1">
-        <v>15</v>
-      </c>
-      <c r="L41" s="1">
-        <v>4</v>
-      </c>
-      <c r="M41" s="1">
-        <v>4</v>
-      </c>
-      <c r="N41" s="1">
-        <v>4</v>
-      </c>
-      <c r="O41" s="1">
-        <v>10</v>
-      </c>
-      <c r="P41" s="5">
-        <v>16</v>
-      </c>
-      <c r="Q41" s="5">
-        <v>17</v>
-      </c>
-      <c r="R41" s="5">
-        <v>10</v>
-      </c>
-      <c r="S41" s="5">
-        <v>10</v>
-      </c>
-      <c r="T41" s="5">
-        <v>5</v>
-      </c>
-      <c r="U41" s="5">
-        <v>21</v>
-      </c>
-      <c r="V41" s="5">
-        <v>12</v>
-      </c>
-      <c r="W41" s="5">
-        <v>6</v>
       </c>
       <c r="X41" s="5">
         <v>16</v>
       </c>
       <c r="Y41" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z41" s="5">
+        <v>22</v>
+      </c>
+      <c r="AA41" s="5">
         <v>26</v>
       </c>
-      <c r="Z41" s="5">
+      <c r="AB41" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC41" s="5">
+        <v>4</v>
+      </c>
+      <c r="AD41" s="5">
+        <v>4</v>
+      </c>
+      <c r="AE41" s="5">
+        <v>6</v>
+      </c>
+      <c r="AF41" s="5">
+        <v>43</v>
+      </c>
+      <c r="AG41" s="5">
+        <v>43</v>
+      </c>
+      <c r="AH41" s="5">
+        <v>41</v>
+      </c>
+      <c r="AI41" s="5">
+        <v>12</v>
+      </c>
+      <c r="AJ41" s="5">
+        <v>4</v>
+      </c>
+      <c r="AK41" s="5">
+        <v>7</v>
+      </c>
+      <c r="AL41" s="5">
+        <v>16</v>
+      </c>
+      <c r="AM41" s="5">
+        <v>11</v>
+      </c>
+      <c r="AN41" s="5">
+        <v>11</v>
+      </c>
+      <c r="AO41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP41" s="5">
+        <v>41</v>
+      </c>
+      <c r="AQ41" s="5">
+        <v>21</v>
+      </c>
+      <c r="AR41" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A42" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="1">
         <v>24</v>
       </c>
-      <c r="AA41" s="5">
+      <c r="C42" s="1">
+        <v>7</v>
+      </c>
+      <c r="D42" s="1">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2</v>
+      </c>
+      <c r="H42" s="1">
+        <v>6</v>
+      </c>
+      <c r="I42" s="1">
+        <v>17</v>
+      </c>
+      <c r="J42" s="1">
+        <v>29</v>
+      </c>
+      <c r="K42" s="1">
+        <v>25</v>
+      </c>
+      <c r="L42" s="1">
+        <v>24</v>
+      </c>
+      <c r="M42" s="1">
+        <v>24</v>
+      </c>
+      <c r="N42" s="1">
+        <v>24</v>
+      </c>
+      <c r="O42" s="1">
+        <v>40</v>
+      </c>
+      <c r="P42" s="5">
+        <v>48</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>46</v>
+      </c>
+      <c r="R42" s="5">
+        <v>39</v>
+      </c>
+      <c r="S42" s="5">
+        <v>37</v>
+      </c>
+      <c r="T42" s="5">
+        <v>32</v>
+      </c>
+      <c r="U42" s="5">
+        <v>51</v>
+      </c>
+      <c r="V42" s="5">
+        <v>41</v>
+      </c>
+      <c r="W42" s="5">
+        <v>31</v>
+      </c>
+      <c r="X42" s="5">
+        <v>38</v>
+      </c>
+      <c r="Y42" s="5">
+        <v>46</v>
+      </c>
+      <c r="Z42" s="5">
+        <v>43</v>
+      </c>
+      <c r="AA42" s="5">
+        <v>25</v>
+      </c>
+      <c r="AB42" s="5">
+        <v>46</v>
+      </c>
+      <c r="AC42" s="5">
+        <v>47</v>
+      </c>
+      <c r="AD42" s="5">
+        <v>47</v>
+      </c>
+      <c r="AE42" s="5">
+        <v>43</v>
+      </c>
+      <c r="AF42" s="5">
         <v>19</v>
       </c>
-      <c r="AB41" s="5">
+      <c r="AG42" s="5">
+        <v>7</v>
+      </c>
+      <c r="AH42" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI42" s="5">
+        <v>34</v>
+      </c>
+      <c r="AJ42" s="5">
+        <v>47</v>
+      </c>
+      <c r="AK42" s="5">
+        <v>49</v>
+      </c>
+      <c r="AL42" s="5">
+        <v>30</v>
+      </c>
+      <c r="AM42" s="5">
+        <v>39</v>
+      </c>
+      <c r="AN42" s="5">
+        <v>43</v>
+      </c>
+      <c r="AO42" s="5">
+        <v>47</v>
+      </c>
+      <c r="AP42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ42" s="5">
+        <v>43</v>
+      </c>
+      <c r="AR42" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="1">
+        <v>26</v>
+      </c>
+      <c r="C43" s="1">
+        <v>55</v>
+      </c>
+      <c r="D43" s="1">
+        <v>55</v>
+      </c>
+      <c r="E43" s="1">
+        <v>49</v>
+      </c>
+      <c r="F43" s="1">
+        <v>49</v>
+      </c>
+      <c r="G43" s="1">
+        <v>46</v>
+      </c>
+      <c r="H43" s="1">
+        <v>44</v>
+      </c>
+      <c r="I43" s="1">
+        <v>36</v>
+      </c>
+      <c r="J43" s="1">
+        <v>24</v>
+      </c>
+      <c r="K43" s="1">
+        <v>21</v>
+      </c>
+      <c r="L43" s="1">
+        <v>24</v>
+      </c>
+      <c r="M43" s="1">
+        <v>23</v>
+      </c>
+      <c r="N43" s="1">
+        <v>22</v>
+      </c>
+      <c r="O43" s="1">
+        <v>18</v>
+      </c>
+      <c r="P43" s="5">
+        <v>15</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>15</v>
+      </c>
+      <c r="R43" s="5">
+        <v>15</v>
+      </c>
+      <c r="S43" s="5">
+        <v>19</v>
+      </c>
+      <c r="T43" s="5">
+        <v>15</v>
+      </c>
+      <c r="U43" s="5">
+        <v>29</v>
+      </c>
+      <c r="V43" s="5">
+        <v>23</v>
+      </c>
+      <c r="W43" s="5">
         <v>17</v>
       </c>
-      <c r="AC41" s="5">
-        <v>18</v>
-      </c>
-      <c r="AD41" s="5">
-        <v>18</v>
-      </c>
-      <c r="AE41" s="5">
-        <v>14</v>
-      </c>
-      <c r="AF41" s="5">
-        <v>27</v>
-      </c>
-      <c r="AG41" s="5">
-        <v>30</v>
-      </c>
-      <c r="AH41" s="5">
-        <v>28</v>
-      </c>
-      <c r="AI41" s="5">
-        <v>4</v>
-      </c>
-      <c r="AJ41" s="5">
-        <v>18</v>
-      </c>
-      <c r="AK41" s="5">
+      <c r="X43" s="5">
+        <v>20</v>
+      </c>
+      <c r="Y43" s="5">
+        <v>7</v>
+      </c>
+      <c r="Z43" s="5">
+        <v>4</v>
+      </c>
+      <c r="AA43" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB43" s="5">
+        <v>19</v>
+      </c>
+      <c r="AC43" s="5">
         <v>17</v>
       </c>
-      <c r="AL41" s="5">
-        <v>10</v>
-      </c>
-      <c r="AM41" s="5">
-        <v>7</v>
-      </c>
-      <c r="AN41" s="5">
-        <v>17</v>
-      </c>
-      <c r="AO41" s="5">
-        <v>0</v>
-      </c>
-      <c r="AP41" s="5">
-        <v>9</v>
-      </c>
-      <c r="AQ41" s="5">
-        <v>18</v>
-      </c>
-      <c r="AR41" s="5">
-        <v>18</v>
-      </c>
-      <c r="AS41" s="5">
-        <v>26</v>
-      </c>
-      <c r="AT41" s="5">
+      <c r="AD43" s="5">
+        <v>19</v>
+      </c>
+      <c r="AE43" s="5">
+        <v>19</v>
+      </c>
+      <c r="AF43" s="5">
+        <v>22</v>
+      </c>
+      <c r="AG43" s="5">
+        <v>59</v>
+      </c>
+      <c r="AH43" s="5">
+        <v>55</v>
+      </c>
+      <c r="AI43" s="5">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A42" s="1" t="s">
+      <c r="AJ43" s="5">
+        <v>19</v>
+      </c>
+      <c r="AK43" s="5">
+        <v>15</v>
+      </c>
+      <c r="AL43" s="5">
+        <v>25</v>
+      </c>
+      <c r="AM43" s="5">
         <v>24</v>
       </c>
-      <c r="B42" s="1">
-        <v>22</v>
-      </c>
-      <c r="C42" s="1">
-        <v>34</v>
-      </c>
-      <c r="D42" s="1">
-        <v>35</v>
-      </c>
-      <c r="E42" s="1">
-        <v>33</v>
-      </c>
-      <c r="F42" s="1">
-        <v>33</v>
-      </c>
-      <c r="G42" s="1">
-        <v>34</v>
-      </c>
-      <c r="H42" s="1">
-        <v>29</v>
-      </c>
-      <c r="I42" s="1">
-        <v>18</v>
-      </c>
-      <c r="J42" s="1">
+      <c r="AN43" s="5">
         <v>11</v>
       </c>
-      <c r="K42" s="1">
-        <v>19</v>
-      </c>
-      <c r="L42" s="1">
-        <v>5</v>
-      </c>
-      <c r="M42" s="1">
-        <v>3</v>
-      </c>
-      <c r="N42" s="1">
-        <v>3</v>
-      </c>
-      <c r="O42" s="1">
-        <v>5</v>
-      </c>
-      <c r="P42" s="5">
-        <v>11</v>
-      </c>
-      <c r="Q42" s="5">
-        <v>11</v>
-      </c>
-      <c r="R42" s="5">
-        <v>3</v>
-      </c>
-      <c r="S42" s="5">
-        <v>7</v>
-      </c>
-      <c r="T42" s="5">
-        <v>11</v>
-      </c>
-      <c r="U42" s="5">
-        <v>14</v>
-      </c>
-      <c r="V42" s="5">
-        <v>7</v>
-      </c>
-      <c r="W42" s="5">
-        <v>8</v>
-      </c>
-      <c r="X42" s="5">
-        <v>14</v>
-      </c>
-      <c r="Y42" s="5">
-        <v>24</v>
-      </c>
-      <c r="Z42" s="5">
-        <v>21</v>
-      </c>
-      <c r="AA42" s="5">
-        <v>21</v>
-      </c>
-      <c r="AB42" s="5">
-        <v>12</v>
-      </c>
-      <c r="AC42" s="5">
-        <v>12</v>
-      </c>
-      <c r="AD42" s="5">
-        <v>12</v>
-      </c>
-      <c r="AE42" s="5">
-        <v>6</v>
-      </c>
-      <c r="AF42" s="5">
-        <v>34</v>
-      </c>
-      <c r="AG42" s="5">
-        <v>35</v>
-      </c>
-      <c r="AH42" s="5">
-        <v>33</v>
-      </c>
-      <c r="AI42" s="5">
-        <v>3</v>
-      </c>
-      <c r="AJ42" s="5">
-        <v>12</v>
-      </c>
-      <c r="AK42" s="5">
-        <v>11</v>
-      </c>
-      <c r="AL42" s="5">
-        <v>7</v>
-      </c>
-      <c r="AM42" s="5">
-        <v>6</v>
-      </c>
-      <c r="AN42" s="5">
-        <v>21</v>
-      </c>
-      <c r="AO42" s="5">
-        <v>7</v>
-      </c>
-      <c r="AP42" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ42" s="5">
-        <v>14</v>
-      </c>
-      <c r="AR42" s="5">
-        <v>11</v>
-      </c>
-      <c r="AS42" s="5">
-        <v>33</v>
-      </c>
-      <c r="AT42" s="5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="1">
-        <v>20</v>
-      </c>
-      <c r="C43" s="1">
-        <v>42</v>
-      </c>
-      <c r="D43" s="1">
-        <v>42</v>
-      </c>
-      <c r="E43" s="1">
-        <v>37</v>
-      </c>
-      <c r="F43" s="1">
-        <v>37</v>
-      </c>
-      <c r="G43" s="1">
-        <v>37</v>
-      </c>
-      <c r="H43" s="1">
-        <v>32</v>
-      </c>
-      <c r="I43" s="1">
-        <v>25</v>
-      </c>
-      <c r="J43" s="1">
-        <v>16</v>
-      </c>
-      <c r="K43" s="1">
-        <v>18</v>
-      </c>
-      <c r="L43" s="1">
-        <v>14</v>
-      </c>
-      <c r="M43" s="1">
-        <v>13</v>
-      </c>
-      <c r="N43" s="1">
-        <v>12</v>
-      </c>
-      <c r="O43" s="1">
-        <v>9</v>
-      </c>
-      <c r="P43" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q43" s="5">
-        <v>5</v>
-      </c>
-      <c r="R43" s="5">
-        <v>11</v>
-      </c>
-      <c r="S43" s="5">
-        <v>9</v>
-      </c>
-      <c r="T43" s="5">
-        <v>20</v>
-      </c>
-      <c r="U43" s="5">
-        <v>12</v>
-      </c>
-      <c r="V43" s="5">
-        <v>8</v>
-      </c>
-      <c r="W43" s="5">
-        <v>12</v>
-      </c>
-      <c r="X43" s="5">
-        <v>6</v>
-      </c>
-      <c r="Y43" s="5">
-        <v>13</v>
-      </c>
-      <c r="Z43" s="5">
-        <v>12</v>
-      </c>
-      <c r="AA43" s="5">
-        <v>18</v>
-      </c>
-      <c r="AB43" s="5">
-        <v>7</v>
-      </c>
-      <c r="AC43" s="5">
-        <v>9</v>
-      </c>
-      <c r="AD43" s="5">
-        <v>9</v>
-      </c>
-      <c r="AE43" s="5">
-        <v>13</v>
-      </c>
-      <c r="AF43" s="5">
-        <v>43</v>
-      </c>
-      <c r="AG43" s="5">
-        <v>42</v>
-      </c>
-      <c r="AH43" s="5">
-        <v>37</v>
-      </c>
-      <c r="AI43" s="5">
-        <v>13</v>
-      </c>
-      <c r="AJ43" s="5">
-        <v>9</v>
-      </c>
-      <c r="AK43" s="5">
-        <v>5</v>
-      </c>
-      <c r="AL43" s="5">
-        <v>9</v>
-      </c>
-      <c r="AM43" s="5">
-        <v>11</v>
-      </c>
-      <c r="AN43" s="5">
-        <v>21</v>
-      </c>
       <c r="AO43" s="5">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="AP43" s="5">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="AQ43" s="5">
         <v>0</v>
@@ -56560,430 +56324,138 @@
       <c r="AR43" s="5">
         <v>11</v>
       </c>
-      <c r="AS43" s="5">
-        <v>37</v>
-      </c>
-      <c r="AT43" s="5">
-        <v>11</v>
-      </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A44" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="5">
+        <v>14</v>
+      </c>
+      <c r="C44" s="5">
+        <v>32</v>
+      </c>
+      <c r="D44" s="5">
+        <v>33</v>
+      </c>
+      <c r="E44" s="5">
         <v>28</v>
       </c>
-      <c r="B44" s="1">
-        <v>29</v>
-      </c>
-      <c r="C44" s="1">
-        <v>43</v>
-      </c>
-      <c r="D44" s="1">
-        <v>43</v>
-      </c>
-      <c r="E44" s="1">
-        <v>41</v>
-      </c>
-      <c r="F44" s="1">
-        <v>41</v>
-      </c>
-      <c r="G44" s="1">
-        <v>42</v>
-      </c>
-      <c r="H44" s="1">
-        <v>37</v>
-      </c>
-      <c r="I44" s="1">
-        <v>26</v>
-      </c>
-      <c r="J44" s="1">
-        <v>19</v>
-      </c>
-      <c r="K44" s="1">
-        <v>29</v>
-      </c>
-      <c r="L44" s="1">
+      <c r="F44" s="5">
+        <v>28</v>
+      </c>
+      <c r="G44" s="5">
+        <v>28</v>
+      </c>
+      <c r="H44" s="5">
+        <v>23</v>
+      </c>
+      <c r="I44" s="5">
+        <v>16</v>
+      </c>
+      <c r="J44" s="5">
+        <v>8</v>
+      </c>
+      <c r="K44" s="5">
+        <v>12</v>
+      </c>
+      <c r="L44" s="5">
+        <v>8</v>
+      </c>
+      <c r="M44" s="5">
+        <v>7</v>
+      </c>
+      <c r="N44" s="5">
+        <v>7</v>
+      </c>
+      <c r="O44" s="5">
+        <v>9</v>
+      </c>
+      <c r="P44" s="5">
+        <v>12</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>12</v>
+      </c>
+      <c r="R44" s="5">
+        <v>9</v>
+      </c>
+      <c r="S44" s="5">
+        <v>5</v>
+      </c>
+      <c r="T44" s="5">
+        <v>13</v>
+      </c>
+      <c r="U44" s="5">
+        <v>17</v>
+      </c>
+      <c r="V44" s="5">
+        <v>9</v>
+      </c>
+      <c r="W44" s="5">
+        <v>5</v>
+      </c>
+      <c r="X44" s="5">
+        <v>6</v>
+      </c>
+      <c r="Y44" s="5">
+        <v>16</v>
+      </c>
+      <c r="Z44" s="5">
+        <v>13</v>
+      </c>
+      <c r="AA44" s="5">
         <v>14</v>
       </c>
-      <c r="M44" s="1">
+      <c r="AB44" s="5">
+        <v>13</v>
+      </c>
+      <c r="AC44" s="5">
+        <v>15</v>
+      </c>
+      <c r="AD44" s="5">
+        <v>15</v>
+      </c>
+      <c r="AE44" s="5">
         <v>12</v>
       </c>
-      <c r="N44" s="1">
+      <c r="AF44" s="5">
+        <v>33</v>
+      </c>
+      <c r="AG44" s="5">
+        <v>33</v>
+      </c>
+      <c r="AH44" s="5">
+        <v>28</v>
+      </c>
+      <c r="AI44" s="5">
+        <v>7</v>
+      </c>
+      <c r="AJ44" s="5">
+        <v>15</v>
+      </c>
+      <c r="AK44" s="5">
         <v>12</v>
       </c>
-      <c r="O44" s="1">
-        <v>7</v>
-      </c>
-      <c r="P44" s="5">
-        <v>6</v>
-      </c>
-      <c r="Q44" s="5">
-        <v>7</v>
-      </c>
-      <c r="R44" s="5">
-        <v>9</v>
-      </c>
-      <c r="S44" s="5">
-        <v>11</v>
-      </c>
-      <c r="T44" s="5">
-        <v>20</v>
-      </c>
-      <c r="U44" s="5">
-        <v>4</v>
-      </c>
-      <c r="V44" s="5">
-        <v>7</v>
-      </c>
-      <c r="W44" s="5">
+      <c r="AL44" s="5">
+        <v>10</v>
+      </c>
+      <c r="AM44" s="5">
+        <v>10</v>
+      </c>
+      <c r="AN44" s="5">
+        <v>10</v>
+      </c>
+      <c r="AO44" s="5">
         <v>15</v>
       </c>
-      <c r="X44" s="5">
-        <v>16</v>
-      </c>
-      <c r="Y44" s="5">
-        <v>24</v>
-      </c>
-      <c r="Z44" s="5">
-        <v>22</v>
-      </c>
-      <c r="AA44" s="5">
-        <v>26</v>
-      </c>
-      <c r="AB44" s="5">
-        <v>5</v>
-      </c>
-      <c r="AC44" s="5">
-        <v>4</v>
-      </c>
-      <c r="AD44" s="5">
-        <v>4</v>
-      </c>
-      <c r="AE44" s="5">
-        <v>6</v>
-      </c>
-      <c r="AF44" s="5">
-        <v>43</v>
-      </c>
-      <c r="AG44" s="5">
-        <v>43</v>
-      </c>
-      <c r="AH44" s="5">
-        <v>41</v>
-      </c>
-      <c r="AI44" s="5">
-        <v>12</v>
-      </c>
-      <c r="AJ44" s="5">
-        <v>4</v>
-      </c>
-      <c r="AK44" s="5">
-        <v>7</v>
-      </c>
-      <c r="AL44" s="5">
+      <c r="AP44" s="5">
+        <v>28</v>
+      </c>
+      <c r="AQ44" s="5">
         <v>13</v>
       </c>
-      <c r="AM44" s="5">
-        <v>13</v>
-      </c>
-      <c r="AN44" s="5">
-        <v>29</v>
-      </c>
-      <c r="AO44" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP44" s="5">
-        <v>11</v>
-      </c>
-      <c r="AQ44" s="5">
-        <v>11</v>
-      </c>
       <c r="AR44" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS44" s="5">
-        <v>41</v>
-      </c>
-      <c r="AT44" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A45" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="1">
-        <v>24</v>
-      </c>
-      <c r="C45" s="1">
-        <v>7</v>
-      </c>
-      <c r="D45" s="1">
-        <v>7</v>
-      </c>
-      <c r="E45" s="1">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1">
-        <v>0</v>
-      </c>
-      <c r="G45" s="1">
-        <v>2</v>
-      </c>
-      <c r="H45" s="1">
-        <v>6</v>
-      </c>
-      <c r="I45" s="1">
-        <v>17</v>
-      </c>
-      <c r="J45" s="1">
-        <v>29</v>
-      </c>
-      <c r="K45" s="1">
-        <v>25</v>
-      </c>
-      <c r="L45" s="1">
-        <v>24</v>
-      </c>
-      <c r="M45" s="1">
-        <v>24</v>
-      </c>
-      <c r="N45" s="1">
-        <v>24</v>
-      </c>
-      <c r="O45" s="1">
-        <v>40</v>
-      </c>
-      <c r="P45" s="5">
-        <v>48</v>
-      </c>
-      <c r="Q45" s="5">
-        <v>46</v>
-      </c>
-      <c r="R45" s="5">
-        <v>39</v>
-      </c>
-      <c r="S45" s="5">
-        <v>37</v>
-      </c>
-      <c r="T45" s="5">
-        <v>32</v>
-      </c>
-      <c r="U45" s="5">
-        <v>51</v>
-      </c>
-      <c r="V45" s="5">
-        <v>41</v>
-      </c>
-      <c r="W45" s="5">
-        <v>31</v>
-      </c>
-      <c r="X45" s="5">
-        <v>38</v>
-      </c>
-      <c r="Y45" s="5">
-        <v>46</v>
-      </c>
-      <c r="Z45" s="5">
-        <v>43</v>
-      </c>
-      <c r="AA45" s="5">
-        <v>25</v>
-      </c>
-      <c r="AB45" s="5">
-        <v>46</v>
-      </c>
-      <c r="AC45" s="5">
-        <v>47</v>
-      </c>
-      <c r="AD45" s="5">
-        <v>47</v>
-      </c>
-      <c r="AE45" s="5">
-        <v>43</v>
-      </c>
-      <c r="AF45" s="5">
-        <v>19</v>
-      </c>
-      <c r="AG45" s="5">
-        <v>7</v>
-      </c>
-      <c r="AH45" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI45" s="5">
-        <v>34</v>
-      </c>
-      <c r="AJ45" s="5">
-        <v>47</v>
-      </c>
-      <c r="AK45" s="5">
-        <v>49</v>
-      </c>
-      <c r="AL45" s="5">
-        <v>34</v>
-      </c>
-      <c r="AM45" s="5">
-        <v>33</v>
-      </c>
-      <c r="AN45" s="5">
-        <v>16</v>
-      </c>
-      <c r="AO45" s="5">
-        <v>30</v>
-      </c>
-      <c r="AP45" s="5">
-        <v>39</v>
-      </c>
-      <c r="AQ45" s="5">
-        <v>43</v>
-      </c>
-      <c r="AR45" s="5">
-        <v>47</v>
-      </c>
-      <c r="AS45" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT45" s="5">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A46" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="1">
-        <v>26</v>
-      </c>
-      <c r="C46" s="1">
-        <v>55</v>
-      </c>
-      <c r="D46" s="1">
-        <v>55</v>
-      </c>
-      <c r="E46" s="1">
-        <v>49</v>
-      </c>
-      <c r="F46" s="1">
-        <v>49</v>
-      </c>
-      <c r="G46" s="1">
-        <v>46</v>
-      </c>
-      <c r="H46" s="1">
-        <v>44</v>
-      </c>
-      <c r="I46" s="1">
-        <v>36</v>
-      </c>
-      <c r="J46" s="1">
-        <v>24</v>
-      </c>
-      <c r="K46" s="1">
-        <v>21</v>
-      </c>
-      <c r="L46" s="1">
-        <v>24</v>
-      </c>
-      <c r="M46" s="1">
-        <v>23</v>
-      </c>
-      <c r="N46" s="1">
-        <v>22</v>
-      </c>
-      <c r="O46" s="1">
-        <v>18</v>
-      </c>
-      <c r="P46" s="5">
-        <v>15</v>
-      </c>
-      <c r="Q46" s="5">
-        <v>15</v>
-      </c>
-      <c r="R46" s="5">
-        <v>15</v>
-      </c>
-      <c r="S46" s="5">
-        <v>19</v>
-      </c>
-      <c r="T46" s="5">
-        <v>15</v>
-      </c>
-      <c r="U46" s="5">
-        <v>29</v>
-      </c>
-      <c r="V46" s="5">
-        <v>23</v>
-      </c>
-      <c r="W46" s="5">
-        <v>17</v>
-      </c>
-      <c r="X46" s="5">
-        <v>20</v>
-      </c>
-      <c r="Y46" s="5">
-        <v>7</v>
-      </c>
-      <c r="Z46" s="5">
-        <v>4</v>
-      </c>
-      <c r="AA46" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB46" s="5">
-        <v>19</v>
-      </c>
-      <c r="AC46" s="5">
-        <v>17</v>
-      </c>
-      <c r="AD46" s="5">
-        <v>19</v>
-      </c>
-      <c r="AE46" s="5">
-        <v>19</v>
-      </c>
-      <c r="AF46" s="5">
-        <v>22</v>
-      </c>
-      <c r="AG46" s="5">
-        <v>59</v>
-      </c>
-      <c r="AH46" s="5">
-        <v>55</v>
-      </c>
-      <c r="AI46" s="5">
-        <v>23</v>
-      </c>
-      <c r="AJ46" s="5">
-        <v>19</v>
-      </c>
-      <c r="AK46" s="5">
-        <v>15</v>
-      </c>
-      <c r="AL46" s="5">
-        <v>17</v>
-      </c>
-      <c r="AM46" s="5">
-        <v>19</v>
-      </c>
-      <c r="AN46" s="5">
-        <v>27</v>
-      </c>
-      <c r="AO46" s="5">
-        <v>25</v>
-      </c>
-      <c r="AP46" s="5">
-        <v>24</v>
-      </c>
-      <c r="AQ46" s="5">
-        <v>11</v>
-      </c>
-      <c r="AR46" s="5">
-        <v>41</v>
-      </c>
-      <c r="AS46" s="5">
-        <v>49</v>
-      </c>
-      <c r="AT46" s="5">
         <v>0</v>
       </c>
     </row>
@@ -56995,13 +56467,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GC46"/>
+  <dimension ref="A1:GC47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="FO21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="GC48" sqref="GC48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -83734,6 +83206,563 @@
         <v>29</v>
       </c>
     </row>
+    <row r="47" spans="1:185" x14ac:dyDescent="0.15">
+      <c r="A47" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5">
+        <v>0</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0</v>
+      </c>
+      <c r="F47" s="5">
+        <v>0</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0</v>
+      </c>
+      <c r="H47" s="5">
+        <v>0</v>
+      </c>
+      <c r="I47" s="5">
+        <v>0</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0</v>
+      </c>
+      <c r="K47" s="5">
+        <v>0</v>
+      </c>
+      <c r="L47" s="5">
+        <v>0</v>
+      </c>
+      <c r="M47" s="5">
+        <v>0</v>
+      </c>
+      <c r="N47" s="5">
+        <v>0</v>
+      </c>
+      <c r="O47" s="5">
+        <v>0</v>
+      </c>
+      <c r="P47" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="5">
+        <v>0</v>
+      </c>
+      <c r="R47" s="5">
+        <v>0</v>
+      </c>
+      <c r="S47" s="5">
+        <v>0</v>
+      </c>
+      <c r="T47" s="5">
+        <v>0</v>
+      </c>
+      <c r="U47" s="5">
+        <v>0</v>
+      </c>
+      <c r="V47" s="5">
+        <v>0</v>
+      </c>
+      <c r="W47" s="5">
+        <v>0</v>
+      </c>
+      <c r="X47" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BH47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BJ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BK47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BL47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BN47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BT47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BU47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BV47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BW47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BX47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BY47" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CE47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CH47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CI47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CJ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CK47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CL47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CM47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CN47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CO47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CP47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CQ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CR47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CS47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CT47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CU47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CV47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CW47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CX47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CY47" s="5">
+        <v>0</v>
+      </c>
+      <c r="CZ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DC47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DD47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DE47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DF47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DG47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DH47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DI47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DJ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DK47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DL47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DM47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DN47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DO47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DP47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DQ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DR47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DS47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DT47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DU47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DV47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DW47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DX47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DY47" s="5">
+        <v>0</v>
+      </c>
+      <c r="DZ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EC47" s="5">
+        <v>0</v>
+      </c>
+      <c r="ED47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EE47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EF47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EG47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EH47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EI47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EJ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EK47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EL47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EM47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EN47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EO47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EP47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EQ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="ER47" s="5">
+        <v>0</v>
+      </c>
+      <c r="ES47" s="5">
+        <v>0</v>
+      </c>
+      <c r="ET47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EU47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EV47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EW47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EX47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EY47" s="5">
+        <v>0</v>
+      </c>
+      <c r="EZ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FC47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FD47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FE47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FF47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FG47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FH47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FI47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FJ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FK47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FL47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FM47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FN47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FO47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FP47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FQ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FR47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FS47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FT47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FU47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FV47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FW47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FX47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FY47" s="5">
+        <v>0</v>
+      </c>
+      <c r="FZ47" s="5">
+        <v>0</v>
+      </c>
+      <c r="GA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="GB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="GC47" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Teased out a result object. Implemented breadth first search which runs out of memory. Time for threads.
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syd/Dropbox/dev/trip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jazzman/Dropbox/dev/trip/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="40420" windowHeight="20640" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="trip.tab" sheetId="1" r:id="rId1"/>
@@ -50509,11 +50509,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR1" sqref="AR1"/>
+      <selection pane="bottomRight" activeCell="Y34" sqref="Y34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -55059,7 +55059,7 @@
         <v>38</v>
       </c>
       <c r="Y34" s="5">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="Z34" s="5">
         <v>44</v>
@@ -56469,7 +56469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GC44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>